<commit_message>
Major update v1.4.0 release
</commit_message>
<xml_diff>
--- a/server/files/data_template_g7.xlsx
+++ b/server/files/data_template_g7.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Libraries\Documents\PhpstormProjects\app-005\server\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2AC0D6-FC7A-4AE7-B377-210481FD3038}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F39FBD-6136-4322-91DD-03779408066C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24630" windowHeight="11550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2016 Exports" sheetId="1" r:id="rId1"/>
-    <sheet name="2015 Exports" sheetId="2" r:id="rId2"/>
-    <sheet name="2014 Exports" sheetId="4" r:id="rId3"/>
+    <sheet name="2016" sheetId="1" r:id="rId1"/>
+    <sheet name="2015" sheetId="2" r:id="rId2"/>
+    <sheet name="2014" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="11">
   <si>
     <t>Germany</t>
   </si>
@@ -53,7 +53,13 @@
     <t>$bn</t>
   </si>
   <si>
-    <t>Rest of the world</t>
+    <t>Anything below the first blank row will not be parsed.</t>
+  </si>
+  <si>
+    <t>Anything after the first blank column header will not be parsed.</t>
+  </si>
+  <si>
+    <t>Others</t>
   </si>
 </sst>
 </file>
@@ -113,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -130,17 +136,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -187,6 +215,232 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle: Rounded Corners 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0D67B51-6849-41B9-A688-3A6947FD2EEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8486775" y="762000"/>
+          <a:ext cx="3571875" cy="3838575"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>DATA</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> TEMPLATE for chords.bnguyensn.com</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>The application takes data in the form of an n x n matrix, with n &gt;= 2.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>At its current version, the application assumes </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>rows to contain outflows</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>columns to contain inflows</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Negative amounts are not allowed.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>The pre-populated</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> data in this spreadsheet are trade exports of the G7 countries + rest of the world.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Each tab corresponds to a year. Time series navigation is coming in the next version.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -452,20 +706,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="12.7109375" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="11" width="12.7109375" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -490,10 +744,15 @@
         <v>4</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="J1" s="11"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -518,11 +777,15 @@
       <c r="H2" s="4">
         <v>6.25</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="10">
         <v>239.59</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="11"/>
+      <c r="K2" s="8">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -547,11 +810,15 @@
       <c r="H3" s="4">
         <v>7.95</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="10">
         <v>272.67</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="11"/>
+      <c r="K3" s="8">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -576,11 +843,15 @@
       <c r="H4" s="4">
         <v>21</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="10">
         <v>851.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="11"/>
+      <c r="K4" s="8">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -605,11 +876,15 @@
       <c r="H5" s="4">
         <v>8.9</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="10">
         <v>303.77</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="11"/>
+      <c r="K5" s="8">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
@@ -634,11 +909,15 @@
       <c r="H6" s="4">
         <v>65.5</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="10">
         <v>888.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="11"/>
+      <c r="K6" s="8">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -663,11 +942,15 @@
       <c r="H7" s="4">
         <v>8.49</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="10">
         <v>72.170000000000016</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="11"/>
+      <c r="K7" s="8">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
@@ -692,66 +975,127 @@
       <c r="H8" s="4">
         <v>0</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="10">
         <v>495.11</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J8" s="11"/>
+      <c r="K8" s="8">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="9">
+        <v>157.4</v>
+      </c>
+      <c r="C9" s="9">
+        <v>316.89</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1005.04</v>
+      </c>
+      <c r="E9" s="9">
+        <v>281.24</v>
+      </c>
+      <c r="F9" s="9">
+        <v>671.9</v>
+      </c>
+      <c r="G9" s="9">
+        <v>119.33000000000001</v>
+      </c>
+      <c r="H9" s="9">
+        <v>570.91</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="12"/>
+      <c r="K9" s="8">
+        <v>3122.7099999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8">
+        <v>374</v>
+      </c>
+      <c r="C11" s="8">
+        <v>450</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1250</v>
+      </c>
+      <c r="E11" s="8">
+        <v>498</v>
+      </c>
+      <c r="F11" s="8">
+        <v>1320</v>
+      </c>
+      <c r="G11" s="8">
+        <v>365</v>
+      </c>
+      <c r="H11" s="8">
+        <v>689</v>
+      </c>
+      <c r="I11" s="8">
+        <v>3122.7100000000005</v>
+      </c>
+      <c r="J11" s="8"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6">
-        <v>157.4</v>
-      </c>
-      <c r="C9" s="6">
-        <v>316.89</v>
-      </c>
-      <c r="D9" s="6">
-        <v>1005.04</v>
-      </c>
-      <c r="E9" s="6">
-        <v>281.24</v>
-      </c>
-      <c r="F9" s="6">
-        <v>671.9</v>
-      </c>
-      <c r="G9" s="6">
-        <v>119.33000000000001</v>
-      </c>
-      <c r="H9" s="6">
-        <v>570.91</v>
-      </c>
-      <c r="I9" s="4">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:I9">
-    <cfRule type="expression" dxfId="4" priority="6">
+  <conditionalFormatting sqref="B2:J9">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>B2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>J1=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="12.7109375" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="11" width="12.7109375" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -776,10 +1120,15 @@
         <v>4</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -804,11 +1153,15 @@
       <c r="H2" s="4">
         <v>6.29</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="10">
         <v>283.86</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="11"/>
+      <c r="K2" s="8">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -833,11 +1186,15 @@
       <c r="H3" s="4">
         <v>6.81</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="10">
         <v>272.54000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="11"/>
+      <c r="K3" s="8">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -862,11 +1219,15 @@
       <c r="H4" s="4">
         <v>19.3</v>
       </c>
-      <c r="I4" s="4">
-        <v>826.40000000000009</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I4" s="10">
+        <v>826.4</v>
+      </c>
+      <c r="J4" s="11"/>
+      <c r="K4" s="8">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -891,11 +1252,15 @@
       <c r="H5" s="4">
         <v>8.49</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="10">
         <v>308.04000000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="11"/>
+      <c r="K5" s="8">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
@@ -920,11 +1285,15 @@
       <c r="H6" s="4">
         <v>63.5</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="10">
         <v>935.8</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="11"/>
+      <c r="K6" s="8">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -949,11 +1318,15 @@
       <c r="H7" s="4">
         <v>8.3000000000000007</v>
       </c>
-      <c r="I7" s="4">
-        <v>76.670000000000016</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I7" s="10">
+        <v>76.67</v>
+      </c>
+      <c r="J7" s="11"/>
+      <c r="K7" s="8">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
@@ -978,51 +1351,106 @@
       <c r="H8" s="4">
         <v>0</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="10">
         <v>487</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J8" s="11"/>
+      <c r="K8" s="8">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="10">
+        <v>206.37</v>
+      </c>
+      <c r="C9" s="10">
+        <v>316.58999999999997</v>
+      </c>
+      <c r="D9" s="10">
+        <v>988.87</v>
+      </c>
+      <c r="E9" s="10">
+        <v>288.64</v>
+      </c>
+      <c r="F9" s="10">
+        <v>702.2</v>
+      </c>
+      <c r="G9" s="10">
+        <v>129.33000000000001</v>
+      </c>
+      <c r="H9" s="10">
+        <v>558.30999999999995</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="8">
+        <v>3190.31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8">
+        <v>426</v>
+      </c>
+      <c r="C11" s="8">
+        <v>447</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1240</v>
+      </c>
+      <c r="E11" s="8">
+        <v>506</v>
+      </c>
+      <c r="F11" s="8">
+        <v>1380</v>
+      </c>
+      <c r="G11" s="8">
+        <v>390</v>
+      </c>
+      <c r="H11" s="8">
+        <v>671</v>
+      </c>
+      <c r="I11" s="8">
+        <v>3190.3100000000004</v>
+      </c>
+      <c r="J11" s="8"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
-        <v>206.37000000000003</v>
-      </c>
-      <c r="C9" s="4">
-        <v>316.59000000000003</v>
-      </c>
-      <c r="D9" s="4">
-        <v>988.87</v>
-      </c>
-      <c r="E9" s="4">
-        <v>288.64</v>
-      </c>
-      <c r="F9" s="4">
-        <v>702.2</v>
-      </c>
-      <c r="G9" s="4">
-        <v>129.32999999999998</v>
-      </c>
-      <c r="H9" s="4">
-        <v>558.30999999999995</v>
-      </c>
-      <c r="I9" s="4">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:H8 B9:I9">
+  <conditionalFormatting sqref="B2:H8 B9:J9">
     <cfRule type="expression" dxfId="3" priority="3">
       <formula>B2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:J2">
     <cfRule type="expression" dxfId="2" priority="2">
       <formula>I2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I8">
+  <conditionalFormatting sqref="I3:J8">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>I3=0</formula>
     </cfRule>
@@ -1034,20 +1462,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="I8" sqref="B8:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="12.7109375" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="11" width="12.7109375" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1072,10 +1500,15 @@
         <v>4</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1100,11 +1533,15 @@
       <c r="H2" s="4">
         <v>6.53</v>
       </c>
-      <c r="I2" s="4">
-        <v>320.41999999999996</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I2" s="10">
+        <v>320.42</v>
+      </c>
+      <c r="J2" s="11"/>
+      <c r="K2" s="8">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -1129,11 +1566,15 @@
       <c r="H3" s="4">
         <v>7.74</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="10">
         <v>316.61</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="11"/>
+      <c r="K3" s="8">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -1158,11 +1599,15 @@
       <c r="H4" s="4">
         <v>23.2</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="10">
         <v>962.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="11"/>
+      <c r="K4" s="8">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -1187,11 +1632,15 @@
       <c r="H5" s="4">
         <v>10.6</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="10">
         <v>348.65</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="11"/>
+      <c r="K5" s="8">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
@@ -1216,11 +1665,15 @@
       <c r="H6" s="4">
         <v>67.5</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="10">
         <v>978.8</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="11"/>
+      <c r="K6" s="8">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -1245,11 +1698,15 @@
       <c r="H7" s="4">
         <v>10.199999999999999</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="10">
         <v>85.32</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="11"/>
+      <c r="K7" s="8">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
@@ -1274,41 +1731,96 @@
       <c r="H8" s="4">
         <v>0</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="10">
         <v>501.15</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J8" s="11"/>
+      <c r="K8" s="8">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="10">
+        <v>238</v>
+      </c>
+      <c r="C9" s="10">
+        <v>363.45</v>
+      </c>
+      <c r="D9" s="10">
+        <v>1126.97</v>
+      </c>
+      <c r="E9" s="10">
+        <v>321.55</v>
+      </c>
+      <c r="F9" s="10">
+        <v>737.9</v>
+      </c>
+      <c r="G9" s="10">
+        <v>161.94999999999999</v>
+      </c>
+      <c r="H9" s="10">
+        <v>563.23</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="8">
+        <v>3513.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8">
+        <v>473</v>
+      </c>
+      <c r="C11" s="8">
+        <v>510</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1410</v>
+      </c>
+      <c r="E11" s="8">
+        <v>571</v>
+      </c>
+      <c r="F11" s="8">
+        <v>1450</v>
+      </c>
+      <c r="G11" s="8">
+        <v>448</v>
+      </c>
+      <c r="H11" s="8">
+        <v>689</v>
+      </c>
+      <c r="I11" s="8">
+        <v>3513.05</v>
+      </c>
+      <c r="J11" s="8"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
-        <v>238</v>
-      </c>
-      <c r="C9" s="4">
-        <v>363.45</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1126.97</v>
-      </c>
-      <c r="E9" s="4">
-        <v>321.54999999999995</v>
-      </c>
-      <c r="F9" s="4">
-        <v>737.9</v>
-      </c>
-      <c r="G9" s="4">
-        <v>161.94999999999999</v>
-      </c>
-      <c r="H9" s="4">
-        <v>563.23</v>
-      </c>
-      <c r="I9" s="4">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:I9">
+  <conditionalFormatting sqref="B2:J9">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>B2=0</formula>
     </cfRule>

</xml_diff>